<commit_message>
updated code w.r.t program creation pom
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybrid/testdatas/testdata.xlsx
+++ b/src/main/java/com/hybrid/testdatas/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Eclipse Projects\Framework\src\main\java\com\hybrid\testdatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84496FB-4DA8-446E-94FB-C9A936F150BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2011A-9001-4A8F-ABAC-7DF496184211}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>progDesc</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>New Business</t>
+  </si>
+  <si>
+    <t>310307356</t>
+  </si>
+  <si>
+    <t>320069738</t>
   </si>
 </sst>
 </file>
@@ -108,12 +114,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,7 +405,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,11 +458,11 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2">
-        <v>310307356</v>
-      </c>
-      <c r="G2" s="2">
-        <v>310259920</v>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>